<commit_message>
Update contents of Model and OEM in Compile_Options.xlsx
</commit_message>
<xml_diff>
--- a/Compile_Options.xlsx
+++ b/Compile_Options.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -101,10 +101,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Remark</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Sub Model</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -113,10 +109,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Remark</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>SUB_OEM</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -165,7 +157,51 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DAEJI P&amp;I</t>
+    <t>Remarks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- Integrated Monitor DVR
+- Hi3531D
+- 8 channel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- Mobile DVR, Satandalone
+- Hi3521
+- 4 channel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- DAEJI P&amp;I
+- 대지정공(주)
+- 특장차 업체</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- Eastern Mastec
+- 국내영업팀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- Eastern Mastec
+- 해외영업팀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- Mobile DVR, Satandalone
+- Hi3521
+- 4 channel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- Mobile DVR, Satandalone
+- Hi3531D
+- 8 channel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DVR</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -239,7 +275,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -258,11 +294,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -560,7 +605,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5" customHeight="1"/>
   <cols>
@@ -622,7 +669,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>7</v>
@@ -700,7 +747,7 @@
         <v>11703</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
@@ -906,15 +953,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="14.25" customWidth="1"/>
     <col min="2" max="2" width="19.875" customWidth="1"/>
-    <col min="3" max="3" width="25.125" customWidth="1"/>
+    <col min="3" max="3" width="28.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="33" customHeight="1">
@@ -925,42 +970,52 @@
         <v>17</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="29.25" customHeight="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="51.75" customHeight="1">
       <c r="A2" s="5">
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="29.25" customHeight="1">
+        <v>23</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="51.75" customHeight="1">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" ht="29.25" customHeight="1">
+        <v>23</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="51.75" customHeight="1">
       <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" ht="24.75" customHeight="1">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
+        <v>23</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="51.75" customHeight="1">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1"/>
@@ -973,9 +1028,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
@@ -986,13 +1039,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="38.25" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="32.25" customHeight="1">
@@ -1000,14 +1053,14 @@
         <v>0</v>
       </c>
       <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:3" ht="32.25" customHeight="1">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="C3" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1"/>
@@ -1021,7 +1074,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1033,42 +1086,46 @@
   <sheetData>
     <row r="1" spans="1:3" ht="36" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="33" customHeight="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="59.25" customHeight="1">
       <c r="A2" s="2">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="7"/>
-    </row>
-    <row r="3" spans="1:3" ht="33" customHeight="1">
+      <c r="C2" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="59.25" customHeight="1">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="7"/>
-    </row>
-    <row r="4" spans="1:3" ht="33" customHeight="1">
+      <c r="C3" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="59.25" customHeight="1">
       <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="36" customHeight="1"/>
@@ -1097,13 +1154,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="36.75" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="33" customHeight="1">
@@ -1111,21 +1168,21 @@
         <v>0</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="7"/>
+      <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3" ht="33" customHeight="1">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="7"/>
+      <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:3" ht="33" customHeight="1">
       <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="7"/>
+      <c r="C4" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1"/>
@@ -1148,13 +1205,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="31.5" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="28.5" customHeight="1">
@@ -1162,36 +1219,36 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="7"/>
+        <v>22</v>
+      </c>
+      <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:3" ht="28.5" customHeight="1">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="7"/>
+        <v>25</v>
+      </c>
+      <c r="C3" s="10"/>
     </row>
     <row r="4" spans="1:3" ht="28.5" customHeight="1">
       <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="7"/>
+        <v>26</v>
+      </c>
+      <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:3" ht="28.5" customHeight="1">
       <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="7"/>
+        <v>27</v>
+      </c>
+      <c r="C5" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1"/>

</xml_diff>

<commit_message>
Modify ID of compile
</commit_message>
<xml_diff>
--- a/Compile_Options.xlsx
+++ b/Compile_Options.xlsx
@@ -8,26 +8,27 @@
   </bookViews>
   <sheets>
     <sheet name="CompileOptions" sheetId="1" r:id="rId1"/>
-    <sheet name="Model" sheetId="6" r:id="rId2"/>
-    <sheet name="SUB_Model" sheetId="9" r:id="rId3"/>
-    <sheet name="OEM" sheetId="5" r:id="rId4"/>
-    <sheet name="SUB_OEM" sheetId="8" r:id="rId5"/>
-    <sheet name="Region" sheetId="7" r:id="rId6"/>
+    <sheet name="ID" sheetId="11" r:id="rId2"/>
+    <sheet name="Model" sheetId="6" r:id="rId3"/>
+    <sheet name="SUB_Model" sheetId="9" r:id="rId4"/>
+    <sheet name="OEM" sheetId="5" r:id="rId5"/>
+    <sheet name="SUB_OEM" sheetId="8" r:id="rId6"/>
+    <sheet name="Region" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CompileOptions!$A$1:$J$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Model!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">OEM!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Region!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">SUB_Model!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">SUB_OEM!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Model!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">OEM!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Region!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">SUB_Model!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">SUB_OEM!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -202,6 +203,42 @@
   </si>
   <si>
     <t>DVR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NN (Number)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>YY (Year)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rule</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Model 시트 참조</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모델 타입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TT (Model Type)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제품 출시 년도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>당해년도에 출시한 제품의 연변</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TTYYNN</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -275,7 +312,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -308,6 +345,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -606,7 +649,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5" customHeight="1"/>
@@ -648,7 +691,7 @@
     </row>
     <row r="2" spans="1:10" ht="25.5" customHeight="1">
       <c r="A2" s="2">
-        <v>11700</v>
+        <v>101900</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -680,7 +723,7 @@
     </row>
     <row r="3" spans="1:10" ht="25.5" customHeight="1">
       <c r="A3" s="2">
-        <v>11701</v>
+        <v>101901</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -712,7 +755,7 @@
     </row>
     <row r="4" spans="1:10" ht="25.5" customHeight="1">
       <c r="A4" s="2">
-        <v>11702</v>
+        <v>101902</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>15</v>
@@ -744,7 +787,7 @@
     </row>
     <row r="5" spans="1:10" ht="25.5" customHeight="1">
       <c r="A5" s="2">
-        <v>11703</v>
+        <v>101903</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>31</v>
@@ -951,9 +994,84 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="1" width="19.875" customWidth="1"/>
+    <col min="2" max="2" width="28.5" customWidth="1"/>
+    <col min="3" max="3" width="29.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="30" customHeight="1">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" customHeight="1">
+      <c r="A2" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" customHeight="1">
+      <c r="A3" s="12"/>
+      <c r="B3" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="11"/>
+    </row>
+    <row r="4" spans="1:4" ht="30" customHeight="1">
+      <c r="A4" s="12"/>
+      <c r="B4" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A4"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
@@ -1024,7 +1142,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1069,7 +1187,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -1139,7 +1257,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -1191,7 +1309,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>

</xml_diff>